<commit_message>
I believe I have figured all Chapter 3 stuff out
</commit_message>
<xml_diff>
--- a/NavChap3Problems.xlsx
+++ b/NavChap3Problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28829"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633D75F-DEB1-4F25-A343-DBC051FF460F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC5DCD7-65FB-4CB8-B272-E19D0E1147EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="1512" windowWidth="17280" windowHeight="8880" xr2:uid="{812FC90A-9241-4EAB-8AA0-7FD32A730C6E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{812FC90A-9241-4EAB-8AA0-7FD32A730C6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>a</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>ares</t>
+  </si>
+  <si>
+    <t>=D5+F5*F4</t>
   </si>
 </sst>
 </file>
@@ -136,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301F647B-E9F4-46D9-813A-32ECEB0EC835}">
-  <dimension ref="A3:L23"/>
+  <dimension ref="A2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -487,6 +491,11 @@
     <col min="12" max="12" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
@@ -537,8 +546,8 @@
         <v>15.04</v>
       </c>
       <c r="G5">
-        <f>D5+F5*F4</f>
-        <v>40.434570370370373</v>
+        <f>41+50.73/60</f>
+        <v>41.845500000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -720,19 +729,19 @@
       </c>
       <c r="E13">
         <f>$G$5+D13</f>
-        <v>284.51123703703701</v>
+        <v>285.92216666666667</v>
       </c>
       <c r="H13">
         <f>IF(E13&gt;180,360-E13,E13)</f>
-        <v>75.488762962962994</v>
+        <v>74.077833333333331</v>
       </c>
       <c r="I13">
         <f>INT(H13)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13">
         <f>FIXED(MOD(H13,1)*60,1)+0</f>
-        <v>29.3</v>
+        <v>4.7</v>
       </c>
       <c r="K13" t="str">
         <f>IF(E13&gt;180,"E","W")</f>
@@ -740,7 +749,7 @@
       </c>
       <c r="L13" t="str">
         <f>I13&amp;"° "&amp;J13&amp;"' "&amp;K13</f>
-        <v>75° 29.3' E</v>
+        <v>74° 4.7' E</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -756,27 +765,27 @@
       </c>
       <c r="E14">
         <f>$G$5+D14</f>
-        <v>153.48123703703703</v>
+        <v>154.89216666666667</v>
       </c>
       <c r="H14">
         <f>IF(E14&gt;180,360-E14,E14)</f>
-        <v>153.48123703703703</v>
+        <v>154.89216666666667</v>
       </c>
       <c r="I14">
         <f>INT(H14)</f>
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J14">
         <f>FIXED(MOD(H14,1)*60,1)+0</f>
-        <v>28.9</v>
+        <v>53.5</v>
       </c>
       <c r="K14" t="str">
         <f>IF(E14&gt;180,"E","W")</f>
         <v>W</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" ref="L13:L14" si="0">I14&amp;"° "&amp;J14&amp;"' "&amp;K14</f>
-        <v>153° 28.9' W</v>
+        <f t="shared" ref="L14" si="0">I14&amp;"° "&amp;J14&amp;"' "&amp;K14</f>
+        <v>154° 53.5' W</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>